<commit_message>
Upload Excel file CV Discount Check Master File 03.08.2025.xlsx
</commit_message>
<xml_diff>
--- a/Data/Discount_Cheker/CV Discount Check Master File 03.08.2025.xlsx
+++ b/Data/Discount_Cheker/CV Discount Check Master File 03.08.2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auditor RSM Data\To be Consider\08 Aug-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091545B0-C2CD-4110-BA48-F817BDDD35C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8DC7A0-51B0-491E-A5B5-E99655AE90A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9C2300AC-C402-454B-B7CF-00A24C218261}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -984,7 +984,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1004,8 +1004,6 @@
     <xf numFmtId="43" fontId="7" fillId="7" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="7" fillId="7" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="7" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1078,6 +1076,9 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1114,6 +1115,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,15 +1129,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1568,612 +1566,613 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" ht="18.75">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="18.75">
-      <c r="A5" s="13"/>
-      <c r="B5" s="46" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="30">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C5,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>1074002</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="52" t="s">
+        <v>842000</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:15" ht="18.75">
-      <c r="A6" s="13"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="31" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="31">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C6,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>10740</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="26">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="24">
         <v>1</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
     </row>
     <row r="7" spans="1:15" ht="18.75">
-      <c r="A7" s="13"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="31" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C7,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>56908</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="26">
+        <v>49328</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="24">
         <v>2</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" ht="18.75">
-      <c r="A8" s="13"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="31" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C8,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>53244</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="53">
+        <v>42319</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="52">
         <v>3</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:15" ht="18.75">
-      <c r="A9" s="13"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="31" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C9,Sheet1!$B$2:$P$2,0),0),"")</f>
         <v>1519</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:15" ht="18.75">
-      <c r="A10" s="13"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="31" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C10,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>37590</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="53">
+        <v>21050</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="52">
         <v>4</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
     </row>
     <row r="11" spans="1:15" ht="18.75">
-      <c r="A11" s="13"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="31" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C11,Sheet1!$B$2:$P$2,0),0),"")</f>
         <v>3500</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="31" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="32">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C12,Sheet1!$B$2:$P$2,0),0),"")</f>
         <v>12000</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" ht="18.75" hidden="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="28" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="33">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C13,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>1249503</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+        <v>971716</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="1:15" ht="19.5" hidden="1" thickBot="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="29" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C14,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>1211913</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+        <v>950666</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="48" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="35">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C15,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>23000</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+        <v>40000</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:15" ht="39.75" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="24" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="38" t="str">
+      <c r="D16" s="36" t="str">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C16,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>50% INSURANCE FREE + 12K ACCESSORIES PACK FREE + RSA FREE</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-    </row>
-    <row r="17" spans="1:15" ht="39.75" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="63" t="s">
+        <v>100% INSURANCE FREE + RSA FREE</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15" ht="18.75">
+      <c r="A17" s="11"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="36" t="str">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C17,Sheet1!$B$2:$P$2,0),0),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
+        <v>Any Accessories Package from List @ 30%</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="25" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="37">
         <f>IFERROR(VLOOKUP($D$3,Sheet1!$B$2:$P$45,MATCH(Report!$C18,Sheet1!$B$2:$P$2,0),0),"")</f>
         <v>40000</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F5:G9">
     <sortCondition ref="F5:F9"/>
   </sortState>
@@ -2214,50 +2213,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="16" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="16" customWidth="1"/>
-    <col min="8" max="12" width="13.7109375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="16" customWidth="1"/>
-    <col min="14" max="14" width="41.28515625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="40.140625" style="16" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="16" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="32.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="14" customWidth="1"/>
+    <col min="8" max="12" width="13.7109375" style="14" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="14" customWidth="1"/>
+    <col min="14" max="14" width="41.28515625" style="14" customWidth="1"/>
+    <col min="15" max="15" width="40.140625" style="14" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="14" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="61"/>
     </row>
     <row r="2" spans="1:16" ht="75.75" thickBot="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2290,24 +2289,24 @@
       <c r="L2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="15" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="8">
@@ -2320,7 +2319,7 @@
         <v>49328</v>
       </c>
       <c r="F3" s="9">
-        <v>42368</v>
+        <v>42319</v>
       </c>
       <c r="G3" s="9">
         <v>1519</v>
@@ -2335,1631 +2334,1631 @@
         <v>12000</v>
       </c>
       <c r="K3" s="9">
-        <v>971765</v>
+        <v>971716</v>
       </c>
       <c r="L3" s="10">
-        <v>950715</v>
-      </c>
-      <c r="M3" s="19">
+        <v>950666</v>
+      </c>
+      <c r="M3" s="17">
         <v>40000</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="41" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="8">
         <v>832001</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>49001</v>
       </c>
-      <c r="F4" s="11">
-        <v>42800</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="9">
+        <v>41850</v>
+      </c>
+      <c r="G4" s="9">
         <v>1519</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>20800</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>3500</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>12000</v>
       </c>
-      <c r="K4" s="11">
-        <v>961621</v>
-      </c>
-      <c r="L4" s="12">
-        <v>940821</v>
-      </c>
-      <c r="M4" s="19">
+      <c r="K4" s="9">
+        <v>960671</v>
+      </c>
+      <c r="L4" s="10">
+        <v>939871</v>
+      </c>
+      <c r="M4" s="17">
         <v>40000</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="41" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="8">
         <v>867001</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>50143</v>
       </c>
-      <c r="F5" s="11">
-        <v>43540</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="F5" s="9">
+        <v>43491</v>
+      </c>
+      <c r="G5" s="9">
         <v>1519</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>21675</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>3500</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <v>12000</v>
       </c>
-      <c r="K5" s="11">
-        <v>999378</v>
-      </c>
-      <c r="L5" s="12">
-        <v>977703</v>
-      </c>
-      <c r="M5" s="19">
+      <c r="K5" s="9">
+        <v>999329</v>
+      </c>
+      <c r="L5" s="10">
+        <v>977654</v>
+      </c>
+      <c r="M5" s="17">
         <v>40000</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="41" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="8">
         <v>872000</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>50309</v>
       </c>
-      <c r="F6" s="11">
-        <v>43775</v>
-      </c>
-      <c r="G6" s="11">
+      <c r="F6" s="9">
+        <v>43725</v>
+      </c>
+      <c r="G6" s="9">
         <v>1519</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>21800</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>3500</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>12000</v>
       </c>
-      <c r="K6" s="11">
-        <v>1004903</v>
-      </c>
-      <c r="L6" s="12">
-        <v>983103</v>
-      </c>
-      <c r="M6" s="19">
+      <c r="K6" s="9">
+        <v>1004853</v>
+      </c>
+      <c r="L6" s="10">
+        <v>983053</v>
+      </c>
+      <c r="M6" s="17">
         <v>40000</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="8">
         <v>882000</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>50634</v>
       </c>
-      <c r="F7" s="11">
-        <v>44243</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="F7" s="9">
+        <v>44194</v>
+      </c>
+      <c r="G7" s="9">
         <v>1519</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>22050</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="9">
         <v>3500</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="9">
         <v>12000</v>
       </c>
-      <c r="K7" s="11">
-        <v>1015946</v>
-      </c>
-      <c r="L7" s="12">
-        <v>993896</v>
-      </c>
-      <c r="M7" s="19">
+      <c r="K7" s="9">
+        <v>1015897</v>
+      </c>
+      <c r="L7" s="10">
+        <v>993847</v>
+      </c>
+      <c r="M7" s="17">
         <v>40000</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="8">
         <v>862001</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>50035</v>
       </c>
-      <c r="F8" s="11">
-        <v>43306</v>
-      </c>
-      <c r="G8" s="11">
+      <c r="F8" s="9">
+        <v>43256</v>
+      </c>
+      <c r="G8" s="9">
         <v>1519</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>21550</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>3500</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <v>12000</v>
       </c>
-      <c r="K8" s="11">
-        <v>993911</v>
-      </c>
-      <c r="L8" s="12">
-        <v>972361</v>
-      </c>
-      <c r="M8" s="19">
+      <c r="K8" s="9">
+        <v>993861</v>
+      </c>
+      <c r="L8" s="10">
+        <v>972311</v>
+      </c>
+      <c r="M8" s="17">
         <v>40000</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="8">
         <v>865001</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>0</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>51112</v>
       </c>
-      <c r="F9" s="11">
-        <v>43447</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="F9" s="9">
+        <v>43397</v>
+      </c>
+      <c r="G9" s="9">
         <v>1519</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>12975</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="9">
         <v>3500</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <v>12000</v>
       </c>
-      <c r="K9" s="11">
-        <v>989554</v>
-      </c>
-      <c r="L9" s="12">
-        <v>976579</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="K9" s="9">
+        <v>989504</v>
+      </c>
+      <c r="L9" s="10">
+        <v>976529</v>
+      </c>
+      <c r="M9" s="17">
         <v>70000</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="O9" s="20" t="s">
+      <c r="O9" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="8">
         <v>999000</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>54620</v>
       </c>
-      <c r="F10" s="11">
-        <v>49728</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="F10" s="9">
+        <v>49678</v>
+      </c>
+      <c r="G10" s="9">
         <v>1519</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>24975</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>3500</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="9">
         <v>12000</v>
       </c>
-      <c r="K10" s="11">
-        <v>1145342</v>
-      </c>
-      <c r="L10" s="12">
-        <v>1120367</v>
-      </c>
-      <c r="M10" s="19">
+      <c r="K10" s="9">
+        <v>1145292</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1120317</v>
+      </c>
+      <c r="M10" s="17">
         <v>20000</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="8">
         <v>1049000</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>10490</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <v>56163</v>
       </c>
-      <c r="F11" s="11">
-        <v>52072</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="F11" s="9">
+        <v>52022</v>
+      </c>
+      <c r="G11" s="9">
         <v>1519</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <v>36715</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <v>3500</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="9">
         <v>12000</v>
       </c>
-      <c r="K11" s="11">
-        <v>1221459</v>
-      </c>
-      <c r="L11" s="12">
-        <v>1184744</v>
-      </c>
-      <c r="M11" s="19">
+      <c r="K11" s="9">
+        <v>1221409</v>
+      </c>
+      <c r="L11" s="10">
+        <v>1184694</v>
+      </c>
+      <c r="M11" s="17">
         <v>25000</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="8">
         <v>1010000</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>10100</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <v>54887</v>
       </c>
-      <c r="F12" s="11">
-        <v>50594</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="F12" s="9">
+        <v>50194</v>
+      </c>
+      <c r="G12" s="9">
         <v>1519</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>35350</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>3500</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <v>12000</v>
       </c>
-      <c r="K12" s="11">
-        <v>1177950</v>
-      </c>
-      <c r="L12" s="12">
-        <v>1142600</v>
-      </c>
-      <c r="M12" s="19">
+      <c r="K12" s="9">
+        <v>1177550</v>
+      </c>
+      <c r="L12" s="10">
+        <v>1142200</v>
+      </c>
+      <c r="M12" s="17">
         <v>35000</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O12" s="20"/>
-      <c r="P12" s="19">
+      <c r="O12" s="18"/>
+      <c r="P12" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="8">
         <v>983000</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>54007</v>
       </c>
-      <c r="F13" s="11">
-        <v>50228</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="F13" s="9">
+        <v>49528</v>
+      </c>
+      <c r="G13" s="9">
         <v>1519</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="9">
         <v>24575</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="9">
         <v>3500</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <v>12000</v>
       </c>
-      <c r="K13" s="11">
-        <v>1128829</v>
-      </c>
-      <c r="L13" s="12">
-        <v>1104254</v>
-      </c>
-      <c r="M13" s="19">
+      <c r="K13" s="9">
+        <v>1128129</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1103554</v>
+      </c>
+      <c r="M13" s="17">
         <v>35000</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O13" s="20"/>
-      <c r="P13" s="19">
+      <c r="O13" s="18"/>
+      <c r="P13" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="8">
         <v>1040000</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>10400</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="9">
         <v>55868</v>
       </c>
-      <c r="F14" s="11">
-        <v>52000</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="F14" s="9">
+        <v>51600</v>
+      </c>
+      <c r="G14" s="9">
         <v>1519</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="9">
         <v>36400</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="9">
         <v>3500</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="9">
         <v>12000</v>
       </c>
-      <c r="K14" s="11">
-        <v>1211687</v>
-      </c>
-      <c r="L14" s="12">
-        <v>1175287</v>
-      </c>
-      <c r="M14" s="19">
+      <c r="K14" s="9">
+        <v>1211287</v>
+      </c>
+      <c r="L14" s="10">
+        <v>1174887</v>
+      </c>
+      <c r="M14" s="17">
         <v>35000</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O14" s="20"/>
-      <c r="P14" s="19">
+      <c r="O14" s="18"/>
+      <c r="P14" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="8">
         <v>1055000</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>10550</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="9">
         <v>56357</v>
       </c>
-      <c r="F15" s="11">
-        <v>52703</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="F15" s="9">
+        <v>52303</v>
+      </c>
+      <c r="G15" s="9">
         <v>1519</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="9">
         <v>36925</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="9">
         <v>3500</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="9">
         <v>12000</v>
       </c>
-      <c r="K15" s="11">
-        <v>1228555</v>
-      </c>
-      <c r="L15" s="12">
-        <v>1191630</v>
-      </c>
-      <c r="M15" s="19">
+      <c r="K15" s="9">
+        <v>1228155</v>
+      </c>
+      <c r="L15" s="10">
+        <v>1191230</v>
+      </c>
+      <c r="M15" s="17">
         <v>35000</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O15" s="20"/>
-      <c r="P15" s="19">
+      <c r="O15" s="18"/>
+      <c r="P15" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="8">
         <v>1037000</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>10370</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="9">
         <v>55744</v>
       </c>
-      <c r="F16" s="11">
-        <v>51859</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="F16" s="9">
+        <v>51459</v>
+      </c>
+      <c r="G16" s="9">
         <v>1519</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="9">
         <v>36295</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="9">
         <v>3500</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="9">
         <v>12000</v>
       </c>
-      <c r="K16" s="11">
-        <v>1208287</v>
-      </c>
-      <c r="L16" s="12">
-        <v>1171992</v>
-      </c>
-      <c r="M16" s="19">
+      <c r="K16" s="9">
+        <v>1207887</v>
+      </c>
+      <c r="L16" s="10">
+        <v>1171592</v>
+      </c>
+      <c r="M16" s="17">
         <v>35000</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="N16" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="19">
+      <c r="O16" s="18"/>
+      <c r="P16" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="41" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="8">
         <v>1035000</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>10350</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="9">
         <v>55702</v>
       </c>
-      <c r="F17" s="11">
-        <v>51766</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="F17" s="9">
+        <v>51366</v>
+      </c>
+      <c r="G17" s="9">
         <v>1519</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="9">
         <v>36225</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="9">
         <v>3500</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="9">
         <v>12000</v>
       </c>
-      <c r="K17" s="11">
-        <v>1206062</v>
-      </c>
-      <c r="L17" s="12">
-        <v>1169837</v>
-      </c>
-      <c r="M17" s="19">
+      <c r="K17" s="9">
+        <v>1205662</v>
+      </c>
+      <c r="L17" s="10">
+        <v>1169437</v>
+      </c>
+      <c r="M17" s="17">
         <v>35000</v>
       </c>
-      <c r="N17" s="21" t="s">
+      <c r="N17" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="19">
+      <c r="O17" s="18"/>
+      <c r="P17" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="8">
         <v>1065000</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>10650</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="9">
         <v>56612</v>
       </c>
-      <c r="F18" s="11">
-        <v>53172</v>
-      </c>
-      <c r="G18" s="11">
+      <c r="F18" s="9">
+        <v>52772</v>
+      </c>
+      <c r="G18" s="9">
         <v>1519</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="9">
         <v>37275</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="9">
         <v>3500</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="9">
         <v>12000</v>
       </c>
-      <c r="K18" s="11">
-        <v>1239728</v>
-      </c>
-      <c r="L18" s="12">
-        <v>1202453</v>
-      </c>
-      <c r="M18" s="19">
+      <c r="K18" s="9">
+        <v>1239328</v>
+      </c>
+      <c r="L18" s="10">
+        <v>1202053</v>
+      </c>
+      <c r="M18" s="17">
         <v>35000</v>
       </c>
-      <c r="N18" s="21" t="s">
+      <c r="N18" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="19">
+      <c r="O18" s="18"/>
+      <c r="P18" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="41" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="8">
         <v>1065000</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>10650</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="9">
         <v>56612</v>
       </c>
-      <c r="F19" s="11">
-        <v>53172</v>
-      </c>
-      <c r="G19" s="11">
+      <c r="F19" s="9">
+        <v>52772</v>
+      </c>
+      <c r="G19" s="9">
         <v>1519</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="9">
         <v>37275</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="9">
         <v>3500</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="9">
         <v>12000</v>
       </c>
-      <c r="K19" s="11">
-        <v>1239728</v>
-      </c>
-      <c r="L19" s="12">
-        <v>1202453</v>
-      </c>
-      <c r="M19" s="19">
+      <c r="K19" s="9">
+        <v>1239328</v>
+      </c>
+      <c r="L19" s="10">
+        <v>1202053</v>
+      </c>
+      <c r="M19" s="17">
         <v>28000</v>
       </c>
-      <c r="N19" s="21" t="s">
+      <c r="N19" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="19">
+      <c r="O19" s="18"/>
+      <c r="P19" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="41" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="8">
         <v>1049001</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>10490</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="9">
         <v>56170</v>
       </c>
-      <c r="F20" s="11">
-        <v>52422</v>
-      </c>
-      <c r="G20" s="11">
+      <c r="F20" s="9">
+        <v>52022</v>
+      </c>
+      <c r="G20" s="9">
         <v>1519</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="9">
         <v>36715</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="9">
         <v>3500</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <v>12000</v>
       </c>
-      <c r="K20" s="11">
-        <v>1221817</v>
-      </c>
-      <c r="L20" s="12">
-        <v>1185102</v>
-      </c>
-      <c r="M20" s="19">
+      <c r="K20" s="9">
+        <v>1221417</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1184702</v>
+      </c>
+      <c r="M20" s="17">
         <v>35000</v>
       </c>
-      <c r="N20" s="21" t="s">
+      <c r="N20" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="19">
+      <c r="O20" s="18"/>
+      <c r="P20" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="41" t="s">
         <v>78</v>
       </c>
       <c r="C21" s="8">
         <v>1119000</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>11190</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="9">
         <v>58415</v>
       </c>
-      <c r="F21" s="11">
-        <v>55703</v>
-      </c>
-      <c r="G21" s="11">
+      <c r="F21" s="9">
+        <v>55303</v>
+      </c>
+      <c r="G21" s="9">
         <v>1519</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="9">
         <v>27975</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="9">
         <v>3500</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="9">
         <v>12000</v>
       </c>
-      <c r="K21" s="11">
-        <v>1289302</v>
-      </c>
-      <c r="L21" s="12">
-        <v>1261327</v>
-      </c>
-      <c r="M21" s="19">
+      <c r="K21" s="9">
+        <v>1288902</v>
+      </c>
+      <c r="L21" s="10">
+        <v>1260927</v>
+      </c>
+      <c r="M21" s="17">
         <v>70000</v>
       </c>
-      <c r="N21" s="21" t="s">
+      <c r="N21" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="O21" s="20"/>
-      <c r="P21" s="19">
+      <c r="O21" s="18"/>
+      <c r="P21" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="41" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="8">
         <v>1106000</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>11060</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="9">
         <v>58025</v>
       </c>
-      <c r="F22" s="11">
-        <v>55094</v>
-      </c>
-      <c r="G22" s="11">
+      <c r="F22" s="9">
+        <v>54694</v>
+      </c>
+      <c r="G22" s="9">
         <v>1519</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="9">
         <v>38710</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="9">
         <v>3500</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="9">
         <v>12000</v>
       </c>
-      <c r="K22" s="11">
-        <v>1285908</v>
-      </c>
-      <c r="L22" s="12">
-        <v>1247198</v>
-      </c>
-      <c r="M22" s="19">
+      <c r="K22" s="9">
+        <v>1285508</v>
+      </c>
+      <c r="L22" s="10">
+        <v>1246798</v>
+      </c>
+      <c r="M22" s="17">
         <v>25000</v>
       </c>
-      <c r="N22" s="21" t="s">
+      <c r="N22" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O22" s="20"/>
-      <c r="P22" s="19">
+      <c r="O22" s="18"/>
+      <c r="P22" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="41" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="8">
         <v>1070000</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>10700</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="9">
         <v>56776</v>
       </c>
-      <c r="F23" s="11">
-        <v>54306</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="F23" s="9">
+        <v>53006</v>
+      </c>
+      <c r="G23" s="9">
         <v>1519</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="9">
         <v>37450</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="9">
         <v>3500</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="9">
         <v>12000</v>
       </c>
-      <c r="K23" s="11">
-        <v>1246251</v>
-      </c>
-      <c r="L23" s="12">
-        <v>1208801</v>
-      </c>
-      <c r="M23" s="19">
+      <c r="K23" s="9">
+        <v>1244951</v>
+      </c>
+      <c r="L23" s="10">
+        <v>1207501</v>
+      </c>
+      <c r="M23" s="17">
         <v>25000</v>
       </c>
-      <c r="N23" s="21" t="s">
+      <c r="N23" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O23" s="20"/>
-      <c r="P23" s="19">
+      <c r="O23" s="18"/>
+      <c r="P23" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="41" t="s">
         <v>50</v>
       </c>
       <c r="C24" s="8">
         <v>1132000</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>11320</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="9">
         <v>58873</v>
       </c>
-      <c r="F24" s="11">
-        <v>56313</v>
-      </c>
-      <c r="G24" s="11">
+      <c r="F24" s="9">
+        <v>55913</v>
+      </c>
+      <c r="G24" s="9">
         <v>1519</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="9">
         <v>39620</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="9">
         <v>3500</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="9">
         <v>12000</v>
       </c>
-      <c r="K24" s="11">
-        <v>1315145</v>
-      </c>
-      <c r="L24" s="12">
-        <v>1275525</v>
-      </c>
-      <c r="M24" s="19">
+      <c r="K24" s="9">
+        <v>1314745</v>
+      </c>
+      <c r="L24" s="10">
+        <v>1275125</v>
+      </c>
+      <c r="M24" s="17">
         <v>25000</v>
       </c>
-      <c r="N24" s="21" t="s">
+      <c r="N24" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O24" s="20"/>
-      <c r="P24" s="19">
+      <c r="O24" s="18"/>
+      <c r="P24" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="41" t="s">
         <v>80</v>
       </c>
       <c r="C25" s="8">
         <v>1116000</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>11160</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="9">
         <v>58124</v>
       </c>
-      <c r="F25" s="11">
-        <v>55563</v>
-      </c>
-      <c r="G25" s="11">
+      <c r="F25" s="9">
+        <v>55163</v>
+      </c>
+      <c r="G25" s="9">
         <v>1519</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="9">
         <v>39060</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="9">
         <v>3500</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="9">
         <v>12000</v>
       </c>
-      <c r="K25" s="11">
-        <v>1296926</v>
-      </c>
-      <c r="L25" s="12">
-        <v>1257866</v>
-      </c>
-      <c r="M25" s="19">
+      <c r="K25" s="9">
+        <v>1296526</v>
+      </c>
+      <c r="L25" s="10">
+        <v>1257466</v>
+      </c>
+      <c r="M25" s="17">
         <v>25000</v>
       </c>
-      <c r="N25" s="21" t="s">
+      <c r="N25" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O25" s="20"/>
-      <c r="P25" s="19">
+      <c r="O25" s="18"/>
+      <c r="P25" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="41" t="s">
         <v>82</v>
       </c>
       <c r="C26" s="8">
         <v>1080000</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>10800</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="9">
         <v>57041</v>
       </c>
-      <c r="F26" s="11">
-        <v>53875</v>
-      </c>
-      <c r="G26" s="11">
+      <c r="F26" s="9">
+        <v>53475</v>
+      </c>
+      <c r="G26" s="9">
         <v>1519</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="9">
         <v>37800</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="9">
         <v>3500</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="9">
         <v>12000</v>
       </c>
-      <c r="K26" s="11">
-        <v>1256535</v>
-      </c>
-      <c r="L26" s="12">
-        <v>1218735</v>
-      </c>
-      <c r="M26" s="19">
+      <c r="K26" s="9">
+        <v>1256135</v>
+      </c>
+      <c r="L26" s="10">
+        <v>1218335</v>
+      </c>
+      <c r="M26" s="17">
         <v>25000</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="19">
+      <c r="O26" s="18"/>
+      <c r="P26" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="41" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="8">
         <v>1145999</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>11460</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="9">
         <v>59331</v>
       </c>
-      <c r="F27" s="11">
-        <v>56969</v>
-      </c>
-      <c r="G27" s="11">
+      <c r="F27" s="9">
+        <v>56569</v>
+      </c>
+      <c r="G27" s="9">
         <v>1519</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="9">
         <v>40110</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="9">
         <v>3500</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="9">
         <v>12000</v>
       </c>
-      <c r="K27" s="11">
-        <v>1330888</v>
-      </c>
-      <c r="L27" s="12">
-        <v>1290778</v>
-      </c>
-      <c r="M27" s="19">
+      <c r="K27" s="9">
+        <v>1330488</v>
+      </c>
+      <c r="L27" s="10">
+        <v>1290378</v>
+      </c>
+      <c r="M27" s="17">
         <v>25000</v>
       </c>
-      <c r="N27" s="21" t="s">
+      <c r="N27" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="19">
+      <c r="O27" s="18"/>
+      <c r="P27" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="41" t="s">
         <v>51</v>
       </c>
       <c r="C28" s="8">
         <v>1127000</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>11270</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="9">
         <v>58683</v>
       </c>
-      <c r="F28" s="11">
-        <v>56078</v>
-      </c>
-      <c r="G28" s="11">
+      <c r="F28" s="9">
+        <v>55678</v>
+      </c>
+      <c r="G28" s="9">
         <v>1519</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="9">
         <v>39445</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="9">
         <v>3500</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="9">
         <v>12000</v>
       </c>
-      <c r="K28" s="11">
-        <v>1309495</v>
-      </c>
-      <c r="L28" s="12">
-        <v>1270050</v>
-      </c>
-      <c r="M28" s="19">
+      <c r="K28" s="9">
+        <v>1309095</v>
+      </c>
+      <c r="L28" s="10">
+        <v>1269650</v>
+      </c>
+      <c r="M28" s="17">
         <v>25000</v>
       </c>
-      <c r="N28" s="21" t="s">
+      <c r="N28" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O28" s="20"/>
-      <c r="P28" s="19">
+      <c r="O28" s="18"/>
+      <c r="P28" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="41" t="s">
         <v>71</v>
       </c>
       <c r="C29" s="8">
         <v>1044000</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>10440</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="9">
         <v>56776</v>
       </c>
-      <c r="F29" s="11">
-        <v>52188</v>
-      </c>
-      <c r="G29" s="11">
+      <c r="F29" s="9">
+        <v>51788</v>
+      </c>
+      <c r="G29" s="9">
         <v>1519</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="9">
         <v>26100</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="9">
         <v>3500</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="9">
         <v>12000</v>
       </c>
-      <c r="K29" s="11">
-        <v>1206523</v>
-      </c>
-      <c r="L29" s="12">
-        <v>1180423</v>
-      </c>
-      <c r="M29" s="19">
+      <c r="K29" s="9">
+        <v>1206123</v>
+      </c>
+      <c r="L29" s="10">
+        <v>1180023</v>
+      </c>
+      <c r="M29" s="17">
         <v>70000</v>
       </c>
-      <c r="N29" s="21" t="s">
+      <c r="N29" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="O29" s="20"/>
-      <c r="P29" s="19">
+      <c r="O29" s="18"/>
+      <c r="P29" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="41" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="8">
         <v>965000</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>0</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="9">
         <v>53346</v>
       </c>
-      <c r="F30" s="11">
-        <v>48134</v>
-      </c>
-      <c r="G30" s="11">
+      <c r="F30" s="9">
+        <v>47734</v>
+      </c>
+      <c r="G30" s="9">
         <v>1519</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="9">
         <v>24125</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="9">
         <v>3500</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="9">
         <v>16000</v>
       </c>
-      <c r="K30" s="11">
-        <v>1111624</v>
-      </c>
-      <c r="L30" s="12">
-        <v>1087499</v>
-      </c>
-      <c r="M30" s="19">
+      <c r="K30" s="9">
+        <v>1111224</v>
+      </c>
+      <c r="L30" s="10">
+        <v>1087099</v>
+      </c>
+      <c r="M30" s="17">
         <v>10000</v>
       </c>
-      <c r="N30" s="21" t="s">
+      <c r="N30" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O30" s="20" t="s">
+      <c r="O30" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="8">
         <v>1057000</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>10570</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="9">
         <v>56351</v>
       </c>
-      <c r="F31" s="11">
-        <v>52447</v>
-      </c>
-      <c r="G31" s="11">
+      <c r="F31" s="9">
+        <v>52047</v>
+      </c>
+      <c r="G31" s="9">
         <v>1519</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="9">
         <v>36995</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="9">
         <v>3500</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="9">
         <v>16000</v>
       </c>
-      <c r="K31" s="11">
-        <v>1234382</v>
-      </c>
-      <c r="L31" s="12">
-        <v>1197387</v>
-      </c>
-      <c r="M31" s="19">
+      <c r="K31" s="9">
+        <v>1233982</v>
+      </c>
+      <c r="L31" s="10">
+        <v>1196987</v>
+      </c>
+      <c r="M31" s="17">
         <v>10000</v>
       </c>
-      <c r="N31" s="21" t="s">
+      <c r="N31" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="O31" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="8">
         <v>1087002</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>10870</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="9">
         <v>57333</v>
       </c>
-      <c r="F32" s="11">
-        <v>53853</v>
-      </c>
-      <c r="G32" s="11">
+      <c r="F32" s="9">
+        <v>53453</v>
+      </c>
+      <c r="G32" s="9">
         <v>1519</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="9">
         <v>38045</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="9">
         <v>3500</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="9">
         <v>16000</v>
       </c>
-      <c r="K32" s="11">
-        <v>1268122</v>
-      </c>
-      <c r="L32" s="12">
-        <v>1230077</v>
-      </c>
-      <c r="M32" s="19">
+      <c r="K32" s="9">
+        <v>1267722</v>
+      </c>
+      <c r="L32" s="10">
+        <v>1229677</v>
+      </c>
+      <c r="M32" s="17">
         <v>10000</v>
       </c>
-      <c r="N32" s="21" t="s">
+      <c r="N32" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O32" s="20" t="s">
+      <c r="O32" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="41" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="8">
         <v>1005000</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>10050</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="9">
         <v>54652</v>
       </c>
-      <c r="F33" s="11">
-        <v>50009</v>
-      </c>
-      <c r="G33" s="11">
+      <c r="F33" s="9">
+        <v>49609</v>
+      </c>
+      <c r="G33" s="9">
         <v>1519</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="9">
         <v>35175</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="9">
         <v>3500</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33" s="9">
         <v>14000</v>
       </c>
-      <c r="K33" s="11">
-        <v>1173905</v>
-      </c>
-      <c r="L33" s="12">
-        <v>1138730</v>
-      </c>
-      <c r="M33" s="19">
+      <c r="K33" s="9">
+        <v>1173505</v>
+      </c>
+      <c r="L33" s="10">
+        <v>1138330</v>
+      </c>
+      <c r="M33" s="17">
         <v>10000</v>
       </c>
-      <c r="N33" s="21" t="s">
+      <c r="N33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O33" s="20" t="s">
+      <c r="O33" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="41" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="8">
         <v>1093001</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="9">
         <v>10930</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="9">
         <v>57529</v>
       </c>
-      <c r="F34" s="11">
-        <v>54034</v>
-      </c>
-      <c r="G34" s="11">
+      <c r="F34" s="9">
+        <v>53734</v>
+      </c>
+      <c r="G34" s="9">
         <v>1519</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="9">
         <v>38255</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="9">
         <v>3500</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34" s="9">
         <v>14000</v>
       </c>
-      <c r="K34" s="11">
-        <v>1272768</v>
-      </c>
-      <c r="L34" s="12">
-        <v>1234513</v>
-      </c>
-      <c r="M34" s="19">
+      <c r="K34" s="9">
+        <v>1272468</v>
+      </c>
+      <c r="L34" s="10">
+        <v>1234213</v>
+      </c>
+      <c r="M34" s="17">
         <v>10000</v>
       </c>
-      <c r="N34" s="21" t="s">
+      <c r="N34" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="O34" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="41" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="8">
         <v>1049001</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="9">
         <v>10490</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="9">
         <v>56092</v>
       </c>
-      <c r="F35" s="11">
-        <v>52072</v>
-      </c>
-      <c r="G35" s="11">
+      <c r="F35" s="9">
+        <v>51672</v>
+      </c>
+      <c r="G35" s="9">
         <v>1519</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="9">
         <v>36715</v>
       </c>
-      <c r="I35" s="11">
+      <c r="I35" s="9">
         <v>3500</v>
       </c>
-      <c r="J35" s="11">
+      <c r="J35" s="9">
         <v>12000</v>
       </c>
-      <c r="K35" s="11">
-        <v>1221389</v>
-      </c>
-      <c r="L35" s="12">
-        <v>1184674</v>
-      </c>
-      <c r="M35" s="19">
+      <c r="K35" s="9">
+        <v>1220989</v>
+      </c>
+      <c r="L35" s="10">
+        <v>1184274</v>
+      </c>
+      <c r="M35" s="17">
         <v>23000</v>
       </c>
-      <c r="N35" s="21" t="s">
+      <c r="N35" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O35" s="20"/>
-      <c r="P35" s="19">
+      <c r="O35" s="18"/>
+      <c r="P35" s="17">
         <v>40000</v>
       </c>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="41" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="8">
         <v>1074002</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="9">
         <v>10740</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="9">
         <v>56908</v>
       </c>
-      <c r="F36" s="11">
-        <v>53244</v>
-      </c>
-      <c r="G36" s="11">
+      <c r="F36" s="9">
+        <v>52844</v>
+      </c>
+      <c r="G36" s="9">
         <v>1519</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="9">
         <v>37590</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="9">
         <v>3500</v>
       </c>
-      <c r="J36" s="11">
+      <c r="J36" s="9">
         <v>12000</v>
       </c>
-      <c r="K36" s="11">
-        <v>1249503</v>
-      </c>
-      <c r="L36" s="12">
-        <v>1211913</v>
-      </c>
-      <c r="M36" s="19">
+      <c r="K36" s="9">
+        <v>1249103</v>
+      </c>
+      <c r="L36" s="10">
+        <v>1211513</v>
+      </c>
+      <c r="M36" s="17">
         <v>23000</v>
       </c>
-      <c r="N36" s="21" t="s">
+      <c r="N36" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O36" s="20"/>
-      <c r="P36" s="19">
+      <c r="O36" s="18"/>
+      <c r="P36" s="17">
         <v>40000</v>
       </c>
     </row>
@@ -4002,7 +4001,7 @@
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" ref="C2">TRANSPOSE(_xlfn._xlws.SORT(_xlfn._xlws.FILTER(Vehicle_Model[Variant],ISNUMBER(SEARCH(Report!D3,Vehicle_Model[Variant])),"Not Found")))</f>
-        <v>BOL PIK UP FB 1.3T - BS6.2 - PS AC</v>
+        <v>MAXX CITY 1.3 LX BS6.2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4206,12 +4205,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4438,15 +4434,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9062C800-B5CF-4467-9EC7-2088426858BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{250AA7BD-7B6E-43C6-AED0-1E579093AA92}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4471,10 +4471,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{250AA7BD-7B6E-43C6-AED0-1E579093AA92}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9062C800-B5CF-4467-9EC7-2088426858BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>